<commit_message>
Update with work from laptop
</commit_message>
<xml_diff>
--- a/Bone-Data.xlsx
+++ b/Bone-Data.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\Projects\Galperin-Collisions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyRepos\shared\Galperin-Collisions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720F826-EBA1-40CA-A0CE-B2F558579B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bones" sheetId="1" r:id="rId1"/>
     <sheet name="Joints" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Shoulder_Horizontal_Link</t>
   </si>
@@ -138,12 +148,6 @@
     <t>Shoulder_Sagittal_Rotator</t>
   </si>
   <si>
-    <t>Elbow</t>
-  </si>
-  <si>
-    <t>Wrist</t>
-  </si>
-  <si>
     <t>CMC_I_Wiggle</t>
   </si>
   <si>
@@ -217,12 +221,24 @@
   </si>
   <si>
     <t>DIP_V_Rotator</t>
+  </si>
+  <si>
+    <t>Radius_Link</t>
+  </si>
+  <si>
+    <t>Elbow_Flexion_Rotator</t>
+  </si>
+  <si>
+    <t>Wrist_Flexion_Rotator</t>
+  </si>
+  <si>
+    <t>Elbow_Supination_Rotator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,11 +558,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A32"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +630,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -625,7 +641,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -636,7 +652,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -647,7 +663,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -658,7 +674,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -669,7 +685,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -680,7 +696,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -691,7 +707,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -702,7 +718,7 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -713,7 +729,7 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -724,7 +740,7 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -735,7 +751,7 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -746,7 +762,7 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -757,7 +773,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -768,7 +784,7 @@
         <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -779,7 +795,7 @@
         <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -790,7 +806,7 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -801,7 +817,7 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -812,7 +828,7 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -823,7 +839,7 @@
         <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -834,7 +850,7 @@
         <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -845,7 +861,7 @@
         <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -856,7 +872,7 @@
         <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -867,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -878,7 +894,7 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -889,7 +905,7 @@
         <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -900,9 +916,20 @@
         <v>61</v>
       </c>
       <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
         <v>30</v>
       </c>
-      <c r="C32" t="b">
+      <c r="C33" t="b">
         <v>0</v>
       </c>
     </row>
@@ -913,11 +940,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -972,7 +999,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -981,7 +1008,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -990,7 +1017,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -999,7 +1026,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1008,7 +1035,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1017,7 +1044,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1026,7 +1053,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1035,7 +1062,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1044,7 +1071,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1053,7 +1080,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,7 +1089,7 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1071,7 +1098,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1080,7 +1107,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1116,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1098,7 +1125,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1107,7 +1134,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1143,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1125,7 +1152,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1134,7 +1161,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,7 +1170,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1152,7 +1179,7 @@
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1161,7 +1188,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1170,7 +1197,7 @@
         <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1179,7 +1206,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1215,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1197,7 +1224,16 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>Bones!A32+1</f>
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>